<commit_message>
add tests for coldbrook parsers
</commit_message>
<xml_diff>
--- a/bio_diversity/static/test/parser_test_files/test-electrofishing.xlsx
+++ b/bio_diversity/static/test/parser_test_files/test-electrofishing.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="48">
   <si>
     <t>Year</t>
   </si>
@@ -137,6 +137,33 @@
   </si>
   <si>
     <t>Destination Pond</t>
+  </si>
+  <si>
+    <t>End Tank</t>
+  </si>
+  <si>
+    <t>site</t>
+  </si>
+  <si>
+    <t>End Lat</t>
+  </si>
+  <si>
+    <t>End Long</t>
+  </si>
+  <si>
+    <t>crew lead</t>
+  </si>
+  <si>
+    <t>Settings</t>
+  </si>
+  <si>
+    <t>fishing seconds</t>
+  </si>
+  <si>
+    <t># of salmon collected</t>
+  </si>
+  <si>
+    <t># of salmon observed</t>
   </si>
 </sst>
 </file>
@@ -551,29 +578,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:U5"/>
+  <dimension ref="A2:AD5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="10.28515625" customWidth="1"/>
     <col min="6" max="6" width="10.140625" customWidth="1"/>
-    <col min="7" max="8" width="17.42578125" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.85546875" customWidth="1"/>
-    <col min="14" max="14" width="10.140625" customWidth="1"/>
-    <col min="15" max="15" width="16.42578125" customWidth="1"/>
-    <col min="16" max="16" width="16" customWidth="1"/>
-    <col min="17" max="18" width="15" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16" customWidth="1"/>
-    <col min="20" max="20" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.5703125" customWidth="1"/>
+    <col min="7" max="9" width="17.42578125" customWidth="1"/>
+    <col min="10" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.85546875" customWidth="1"/>
+    <col min="17" max="17" width="11.85546875" customWidth="1"/>
+    <col min="18" max="19" width="10.140625" customWidth="1"/>
+    <col min="20" max="22" width="16.42578125" customWidth="1"/>
+    <col min="23" max="23" width="16" customWidth="1"/>
+    <col min="24" max="26" width="15" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="16" customWidth="1"/>
+    <col min="29" max="29" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>25</v>
       </c>
@@ -586,20 +614,29 @@
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="13" t="s">
+      <c r="I2" s="5"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="13"/>
-      <c r="L2" s="14" t="s">
+      <c r="M2" s="13"/>
+      <c r="N2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="15"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="1"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="1"/>
     </row>
-    <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -625,13 +662,13 @@
         <v>38</v>
       </c>
       <c r="I3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="4" t="s">
-        <v>5</v>
-      </c>
       <c r="K3" s="2" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="L3" s="4" t="s">
         <v>5</v>
@@ -640,31 +677,58 @@
         <v>6</v>
       </c>
       <c r="N3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="R3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="S3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="T3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="U3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="W3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="X3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="Y3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="S3" s="2" t="s">
+      <c r="Z3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="T3" s="2" t="s">
+      <c r="AC3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="AD3" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2021</v>
       </c>
@@ -684,32 +748,51 @@
       <c r="H4" t="s">
         <v>35</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="I4">
+        <v>13</v>
+      </c>
+      <c r="J4" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="1"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="5"/>
-      <c r="N4" s="1" t="s">
+      <c r="K4" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="L4" s="1"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="R4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="P4">
+      <c r="S4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="V4">
         <v>110</v>
       </c>
-      <c r="Q4">
+      <c r="W4">
+        <v>110</v>
+      </c>
+      <c r="X4">
         <v>4</v>
       </c>
-      <c r="R4" s="9">
+      <c r="Y4" s="9">
         <v>1.1000000000000001</v>
       </c>
-      <c r="S4">
+      <c r="Z4" s="9">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="AA4">
         <v>350</v>
       </c>
-      <c r="T4">
+      <c r="AB4">
+        <v>350</v>
+      </c>
+      <c r="AC4">
         <v>500</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2021</v>
       </c>
@@ -730,36 +813,53 @@
       <c r="H5" t="s">
         <v>37</v>
       </c>
-      <c r="J5" s="10">
+      <c r="I5">
+        <v>21</v>
+      </c>
+      <c r="L5" s="10">
         <v>45.549656159192402</v>
       </c>
-      <c r="K5" s="1">
+      <c r="M5" s="1">
         <v>-65.013694691467194</v>
       </c>
-      <c r="L5" s="5"/>
-      <c r="N5" s="1" t="s">
+      <c r="N5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="R5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="P5">
+      <c r="S5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="V5">
         <v>200</v>
       </c>
-      <c r="Q5">
+      <c r="W5">
+        <v>200</v>
+      </c>
+      <c r="X5">
         <v>5</v>
       </c>
-      <c r="R5" s="9">
+      <c r="Y5" s="9">
         <v>1.1000000000000001</v>
       </c>
-      <c r="S5">
+      <c r="Z5" s="9">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="AA5">
         <v>788</v>
       </c>
-      <c r="T5">
+      <c r="AB5">
+        <v>788</v>
+      </c>
+      <c r="AC5">
         <v>500</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="J2:K2"/>
+  <mergeCells count="3">
     <mergeCell ref="L2:M2"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="N2:O2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update electrofishing parser converters and test
</commit_message>
<xml_diff>
--- a/bio_diversity/static/test/parser_test_files/test-electrofishing.xlsx
+++ b/bio_diversity/static/test/parser_test_files/test-electrofishing.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="48">
   <si>
     <t>Year</t>
   </si>
@@ -578,10 +578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AD5"/>
+  <dimension ref="A2:AD6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U3" sqref="U3"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -853,6 +853,42 @@
       </c>
       <c r="AC5">
         <v>500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>2021</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="1">
+        <v>6</v>
+      </c>
+      <c r="D6" s="11"/>
+      <c r="E6" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" t="s">
+        <v>30</v>
+      </c>
+      <c r="L6" s="10">
+        <v>45.549656159192402</v>
+      </c>
+      <c r="M6" s="1">
+        <v>-65.013694691467194</v>
+      </c>
+      <c r="N6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="R6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="U6">
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>